<commit_message>
added ICAO row and column labels
</commit_message>
<xml_diff>
--- a/Assignment 1/Problem 1/demand2020_forecast.xlsx
+++ b/Assignment 1/Problem 1/demand2020_forecast.xlsx
@@ -435,70 +435,112 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="n">
-        <v>19</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>EGLL</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>LFPG</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>EHAM</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>EDDF</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>LEMD</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>LEBL</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>EDDM</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>LIRF</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>EIDW</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>ESSA</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>LPPT</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>EDDT</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>EFHK</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>EPWA</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>EGPH</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>LROP</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>LGIR</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>BIKF</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>LICJ</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>LPMA</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>EGLL</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -562,8 +604,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>LFPG</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>1402.296046910472</v>
@@ -627,8 +671,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>EHAM</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>903.3105174988242</v>
@@ -692,8 +738,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>EDDF</t>
+        </is>
       </c>
       <c r="B5" t="n">
         <v>403.057498103921</v>
@@ -757,8 +805,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>LEMD</t>
+        </is>
       </c>
       <c r="B6" t="n">
         <v>273.3755736372722</v>
@@ -822,8 +872,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>LEBL</t>
+        </is>
       </c>
       <c r="B7" t="n">
         <v>204.7437770486284</v>
@@ -887,8 +939,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>EDDM</t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>383.1364194459669</v>
@@ -952,8 +1006,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>LIRF</t>
+        </is>
       </c>
       <c r="B9" t="n">
         <v>237.7205823810009</v>
@@ -1017,8 +1073,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>EIDW</t>
+        </is>
       </c>
       <c r="B10" t="n">
         <v>863.8536087503611</v>
@@ -1082,8 +1140,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>ESSA</t>
+        </is>
       </c>
       <c r="B11" t="n">
         <v>189.9065122870909</v>
@@ -1147,8 +1207,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>LPPT</t>
+        </is>
       </c>
       <c r="B12" t="n">
         <v>60.6291215196551</v>
@@ -1212,8 +1274,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>EDDT</t>
+        </is>
       </c>
       <c r="B13" t="n">
         <v>636.3766710591717</v>
@@ -1277,8 +1341,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>EFHK</t>
+        </is>
       </c>
       <c r="B14" t="n">
         <v>101.2517083559174</v>
@@ -1342,8 +1408,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>EPWA</t>
+        </is>
       </c>
       <c r="B15" t="n">
         <v>103.3991305324099</v>
@@ -1407,8 +1475,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>EGPH</t>
+        </is>
       </c>
       <c r="B16" t="n">
         <v>365.3717011096231</v>
@@ -1472,8 +1542,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>LROP</t>
+        </is>
       </c>
       <c r="B17" t="n">
         <v>59.43303904024551</v>
@@ -1537,8 +1609,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>LGIR</t>
+        </is>
       </c>
       <c r="B18" t="n">
         <v>12.08691410923005</v>
@@ -1602,8 +1676,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>BIKF</t>
+        </is>
       </c>
       <c r="B19" t="n">
         <v>61.50082926892657</v>
@@ -1667,8 +1743,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>LICJ</t>
+        </is>
       </c>
       <c r="B20" t="n">
         <v>75.7854795463186</v>
@@ -1732,8 +1810,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>LPMA</t>
+        </is>
       </c>
       <c r="B21" t="n">
         <v>22.0347329994961</v>

</xml_diff>